<commit_message>
nucleotide settings and contributed artifacts
</commit_message>
<xml_diff>
--- a/mixs-templates/MigsBa_plus_combinations/MigsBa.xlsx
+++ b/mixs-templates/MigsBa_plus_combinations/MigsBa.xlsx
@@ -719,7 +719,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation sqref="S2:S1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"aerobe,anaerobe,facultative,microaerophilic,microanaerobe,obligate aerobe,obligate anaerobe"</formula1>
     </dataValidation>
@@ -728,6 +728,9 @@
     </dataValidation>
     <dataValidation sqref="Y2:Y1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"other,paired,single,vector"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Z2:Z1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Finished genome,High-quality draft genome,Medium-quality draft genome,Low-quality draft genome,Genome fragment(s)"</formula1>
     </dataValidation>
     <dataValidation sqref="AE2:AE1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"DNA-free PCR mix,distilled water,empty collection device,empty collection tube,phosphate buffer,sterile swab,sterile syringe"</formula1>

</xml_diff>